<commit_message>
Se agrega un spacio para pegar los codigos padres.
</commit_message>
<xml_diff>
--- a/Control Stock Web 2024-07-11.xlsx
+++ b/Control Stock Web 2024-07-11.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,61 +446,89 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10727609001</t>
+          <t>10923690001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Disponible</t>
+          <t xml:space="preserve">Error: </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$ 26.990</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
+          <t>Precio no disponible</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Cantidad de imágenes no disponible</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10923690001</t>
+          <t>10727609001</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Disponible</t>
+          <t xml:space="preserve">Error: </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$ 39.990</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
+          <t>Precio no disponible</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Cantidad de imágenes no disponible</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>10820236005</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Error: </t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Precio no disponible</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Cantidad de imágenes no disponible</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>10842374003</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Disponible</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>$ 12.990</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>3</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Error: </t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Precio no disponible</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Cantidad de imágenes no disponible</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agrega contador de proceso y tiempo
</commit_message>
<xml_diff>
--- a/Control Stock Web 2024-07-11.xlsx
+++ b/Control Stock Web 2024-07-11.xlsx
@@ -446,89 +446,81 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10923690001</t>
+          <t>10962736022</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Error: </t>
+          <t>Disponible</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Precio no disponible</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Cantidad de imágenes no disponible</t>
-        </is>
+          <t>$ 62.990</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10727609001</t>
+          <t>10962389016</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Error: </t>
+          <t>Disponible</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Precio no disponible</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Cantidad de imágenes no disponible</t>
-        </is>
+          <t>$ 165.990</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>10820236005</t>
+          <t>10962389018</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Error: </t>
+          <t>Disponible</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Precio no disponible</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Cantidad de imágenes no disponible</t>
-        </is>
+          <t>$ 165.990</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>10842374003</t>
+          <t>10930745010</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Error: </t>
+          <t>Disponible</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Precio no disponible</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Cantidad de imágenes no disponible</t>
-        </is>
+          <t>$ 182.990</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Este script incluye la función ensure_playwright_browsers_installed que verifica si los navegadores de Playwright están instalados y los instala si es necesario. Ahora, al ejecutar tu script, debería manejar automáticamente la instalación de los navegadores requeridos si no están presentes, y continuar con la ejecución normal del código.
</commit_message>
<xml_diff>
--- a/Control Stock Web 2024-07-11.xlsx
+++ b/Control Stock Web 2024-07-11.xlsx
@@ -466,7 +466,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10962389016</t>
+          <t>10930745010</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -476,11 +476,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$ 165.990</t>
+          <t>$ 182.990</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>10930745010</t>
+          <t>10962389016</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -516,11 +516,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>$ 182.990</t>
+          <t>$ 165.990</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
manejo de errores agregados
</commit_message>
<xml_diff>
--- a/Control Stock Web 2024-07-11.xlsx
+++ b/Control Stock Web 2024-07-11.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10962736022</t>
+          <t>10962389016</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -456,7 +456,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$ 62.990</t>
+          <t>$ 165.990</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -466,7 +466,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10930745010</t>
+          <t>10962389018</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -476,17 +476,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$ 182.990</t>
+          <t>$ 165.990</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>10962389018</t>
+          <t>10930745010</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -496,31 +496,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>$ 165.990</t>
+          <t>$ 182.990</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>10962389016</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Disponible</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>$ 165.990</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>